<commit_message>
placing mass balance matrix + testing
</commit_message>
<xml_diff>
--- a/examples/dev_sandbox/data/mini_grid/placing_matrix_all_components_redo.xlsx
+++ b/examples/dev_sandbox/data/mini_grid/placing_matrix_all_components_redo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjordan\Documents\GitHub\ClearWater-riverine\examples\dev_sandbox\data\mini_grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906D3938-4CF7-4090-9117-203003A1ED34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D288744-0C5D-400C-B306-9BCD7BBC6DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14310" yWindow="-18120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="6" xr2:uid="{0D6685A3-9F3A-4630-99AF-4A1490A22806}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{0D6685A3-9F3A-4630-99AF-4A1490A22806}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram" sheetId="15" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="87">
   <si>
     <t>n+1</t>
   </si>
@@ -297,16 +297,53 @@
   </si>
   <si>
     <t xml:space="preserve">assume everything advecting in </t>
+  </si>
+  <si>
+    <t>essentially to account for "advection" back into that cell? Since there's no upstream.</t>
+  </si>
+  <si>
+    <t>completes the upwinds method but without another cell on the receiving end</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0360132319308030</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>&lt;-- this value (7) is equal to if we had the same volume at t=1</t>
+  </si>
+  <si>
+    <t>initial</t>
+  </si>
+  <si>
+    <t>mb</t>
+  </si>
+  <si>
+    <t>loss</t>
+  </si>
+  <si>
+    <t>increase</t>
+  </si>
+  <si>
+    <t>calculated</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>diff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000%"/>
+    <numFmt numFmtId="170" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +403,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -523,7 +568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -561,15 +606,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -601,7 +647,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>83945</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -650,7 +696,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>83945</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -699,7 +745,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>83945</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -748,7 +794,7 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>83945</xdr:rowOff>
+      <xdr:rowOff>87120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1130,16 +1176,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -1297,16 +1343,16 @@
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -1473,16 +1519,16 @@
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -1610,16 +1656,16 @@
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:23" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -2022,16 +2068,16 @@
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -2426,10 +2472,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1C1EA4-B6EB-4A45-9877-35DDB2F0DB00}">
-  <dimension ref="B5:H7"/>
+  <dimension ref="B5:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2443,14 +2489,18 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6">
-        <f>18.8*10^-9</f>
-        <v>1.8800000000000003E-8</v>
+      <c r="B6" s="5">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H7" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2463,12 +2513,13 @@
   <dimension ref="A1:P52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="J3" sqref="J3:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.08984375" bestFit="1" customWidth="1"/>
@@ -2488,6 +2539,9 @@
       <c r="D2" t="s">
         <v>15</v>
       </c>
+      <c r="K2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
@@ -2505,6 +2559,13 @@
       <c r="G3" t="s">
         <v>19</v>
       </c>
+      <c r="J3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3">
+        <f>C3</f>
+        <v>25.002766000000001</v>
+      </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
@@ -2521,6 +2582,13 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
+      <c r="J4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4">
+        <f>E19*300</f>
+        <v>12.499911000000001</v>
+      </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
@@ -2535,6 +2603,13 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5">
+        <f>E20*-300</f>
+        <v>12.500003999999999</v>
+      </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
@@ -2545,6 +2620,31 @@
       </c>
       <c r="D6" t="s">
         <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6">
+        <f>K3-K4+K5</f>
+        <v>25.002859000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="J7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7">
+        <f>D3</f>
+        <v>25.000551000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="J8" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" s="30">
+        <f>K6-K7</f>
+        <v>2.3079999999993106E-3</v>
       </c>
     </row>
     <row r="10" spans="2:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
@@ -2635,7 +2735,7 @@
       </c>
       <c r="H13">
         <f>Constants!B6</f>
-        <v>1.8800000000000003E-8</v>
+        <v>0</v>
       </c>
       <c r="I13" s="5">
         <v>500002.5</v>
@@ -2676,7 +2776,7 @@
       </c>
       <c r="H14">
         <f>H13</f>
-        <v>1.8800000000000003E-8</v>
+        <v>0</v>
       </c>
       <c r="I14" s="5">
         <v>500002.5</v>
@@ -2790,6 +2890,9 @@
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="E21" t="s">
+        <v>78</v>
+      </c>
       <c r="P21" t="s">
         <v>61</v>
       </c>
@@ -2817,8 +2920,8 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
       <c r="H36" s="6" t="s">
         <v>47</v>
       </c>
@@ -2854,7 +2957,7 @@
       </c>
       <c r="H37" s="6">
         <f>G13*H13/M13</f>
-        <v>1.8800415116121397E-8</v>
+        <v>0</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>3</v>
@@ -2864,7 +2967,7 @@
       </c>
       <c r="K37" s="6">
         <f>G13*H13/M13</f>
-        <v>1.8800415116121397E-8</v>
+        <v>0</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>2</v>
@@ -2893,7 +2996,7 @@
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="H41" s="6">
         <f>G14*H14/M14</f>
-        <v>3.7600839250463518E-8</v>
+        <v>0</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>5</v>
@@ -2903,7 +3006,7 @@
       </c>
       <c r="K41" s="6">
         <f>G14*H14/M14</f>
-        <v>3.7600839250463518E-8</v>
+        <v>0</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>2</v>
@@ -2995,11 +3098,20 @@
       <c r="A49" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
+      <c r="B49" s="6">
+        <f>K37+K41</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="6">
+        <f>H37*-1</f>
+        <v>0</v>
+      </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
+      <c r="F49" s="6">
+        <f>H41*-1</f>
+        <v>0</v>
+      </c>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
       <c r="I49" s="6"/>
@@ -3099,8 +3211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E4236B-66F9-423D-A03D-51068852B328}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3127,7 +3239,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
@@ -3143,9 +3255,16 @@
       <c r="G3" t="s">
         <v>19</v>
       </c>
+      <c r="J3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3">
+        <f>C3</f>
+        <v>25.002766000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="8"/>
       <c r="C4">
         <f>C3/35.315</f>
@@ -3155,9 +3274,16 @@
         <f>D3/35.315</f>
         <v>0.70791924111567328</v>
       </c>
+      <c r="J4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4">
+        <f>E19*300</f>
+        <v>12.499911000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
@@ -3170,9 +3296,16 @@
       <c r="E5" t="s">
         <v>18</v>
       </c>
+      <c r="J5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5">
+        <f>E20*-300</f>
+        <v>-12.499881</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
@@ -3181,6 +3314,31 @@
       </c>
       <c r="D6" t="s">
         <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6">
+        <f>K3-K4+K5</f>
+        <v>2.9740000000000322E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K7">
+        <f>D3</f>
+        <v>25.000167999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="J8" s="30" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" s="30">
+        <f>K6-K7</f>
+        <v>-24.997194</v>
       </c>
     </row>
     <row r="10" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
@@ -3263,7 +3421,7 @@
       </c>
       <c r="H13">
         <f>Constants!B6</f>
-        <v>1.8800000000000003E-8</v>
+        <v>0</v>
       </c>
       <c r="I13" s="5">
         <v>500002.5</v>
@@ -3304,7 +3462,7 @@
       </c>
       <c r="H14">
         <f>H13</f>
-        <v>1.8800000000000003E-8</v>
+        <v>0</v>
       </c>
       <c r="I14" s="5">
         <v>500007.5</v>
@@ -3445,8 +3603,8 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
       <c r="H36" s="6" t="s">
         <v>47</v>
       </c>
@@ -3482,7 +3640,7 @@
       </c>
       <c r="H37" s="6">
         <f>G13*H13/M13</f>
-        <v>1.8800415116121397E-8</v>
+        <v>0</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>2</v>
@@ -3492,7 +3650,7 @@
       </c>
       <c r="K37" s="6">
         <f>G13*H13/M13</f>
-        <v>1.8800415116121397E-8</v>
+        <v>0</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>3</v>
@@ -3521,7 +3679,7 @@
     <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="H41" s="6">
         <f>G14*H14/M14</f>
-        <v>3.7600288772966896E-8</v>
+        <v>0</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>7</v>
@@ -3531,7 +3689,7 @@
       </c>
       <c r="K41" s="6">
         <f>G14*H14/M14</f>
-        <v>3.7600288772966896E-8</v>
+        <v>0</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>3</v>
@@ -3623,13 +3781,22 @@
       <c r="A49" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
+      <c r="B49" s="6">
+        <f>-H37</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="6">
+        <f>K37+K41</f>
+        <v>0</v>
+      </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
+      <c r="H49" s="6">
+        <f>-H41</f>
+        <v>0</v>
+      </c>
       <c r="I49" s="6"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
@@ -3728,8 +3895,556 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3426ABE-99FB-4A09-878D-0022A8B4B1C7}">
   <dimension ref="A1:P52"/>
   <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1796875" customWidth="1"/>
+    <col min="7" max="7" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>21.000109999999999</v>
+      </c>
+      <c r="D3">
+        <v>21.000022999999999</v>
+      </c>
+      <c r="E3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="29">
+        <f>C3-D3</f>
+        <v>8.7000000000614364E-5</v>
+      </c>
+      <c r="G3" s="29">
+        <f>12.500004-F3</f>
+        <v>12.499917</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="27"/>
+      <c r="B4" s="8"/>
+      <c r="C4">
+        <f>C3/35.315</f>
+        <v>0.59465128132521594</v>
+      </c>
+      <c r="D4">
+        <f>D3/35.315</f>
+        <v>0.59464881778281187</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="27"/>
+      <c r="B5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>300</v>
+      </c>
+      <c r="D5">
+        <v>300</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="21"/>
+      <c r="E11" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B12" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>-4.1666679999999998E-2</v>
+      </c>
+      <c r="F13">
+        <v>-8.3331499999999992E-3</v>
+      </c>
+      <c r="G13">
+        <f>E13/F13</f>
+        <v>5.0001116024552541</v>
+      </c>
+      <c r="H13">
+        <f>Constants!B6</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="5">
+        <v>500002.5</v>
+      </c>
+      <c r="J13" s="5">
+        <v>102.5</v>
+      </c>
+      <c r="K13" s="5">
+        <v>500000</v>
+      </c>
+      <c r="L13" s="5">
+        <v>102.5</v>
+      </c>
+      <c r="M13">
+        <f>SQRT((K13-I13)^2-(L13-J13)^2)</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="P14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="P15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B18" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="P18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>-4.1666679999999998E-2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19">
+        <v>-1</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="P19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="H22" s="3"/>
+      <c r="P22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="27" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="28" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="29" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="30" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="H36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="N36" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="O36" s="7"/>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B37" s="8">
+        <f>D3/D5</f>
+        <v>7.0000076666666661E-2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="9">
+        <f>C3/C5*C6</f>
+        <v>7.0000366666666665</v>
+      </c>
+      <c r="F37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" s="6">
+        <f>G13*H13/M13</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K37" s="6">
+        <f>G13*H13/M13</f>
+        <v>0</v>
+      </c>
+      <c r="L37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M37" t="s">
+        <v>45</v>
+      </c>
+      <c r="N37" s="7">
+        <f>E19*G19</f>
+        <v>4.1666679999999998E-2</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="P37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>5</v>
+      </c>
+      <c r="H46">
+        <v>6</v>
+      </c>
+      <c r="I46">
+        <v>7</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8">
+        <f>B37</f>
+        <v>7.0000076666666661E-2</v>
+      </c>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7">
+        <f>N37</f>
+        <v>4.1666679999999998E-2</v>
+      </c>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" s="6">
+        <f>-H37</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6">
+        <f>K37</f>
+        <v>0</v>
+      </c>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51">
+        <f>SUM(B47:B49)</f>
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <f t="shared" ref="C51:I51" si="0">SUM(C47:C49)</f>
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>0.11166675666666666</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M51" s="10">
+        <f>E37</f>
+        <v>7.0000366666666665</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52">
+        <f>B47+B48</f>
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <f t="shared" ref="C52:I52" si="1">C47+C48</f>
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="1"/>
+        <v>0.11166675666666666</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <f>E37</f>
+        <v>7.0000366666666665</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B36:C36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F1D4CD-3FDB-4235-A1C3-31288C66CE2D}">
+  <dimension ref="A1:P52"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3756,15 +4471,15 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
+      <c r="A3" s="27"/>
       <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C3">
-        <v>21.000109999999999</v>
+        <v>20</v>
       </c>
       <c r="D3">
-        <v>21.000022999999999</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>72</v>
@@ -3774,22 +4489,22 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="8"/>
       <c r="C4">
         <f>C3/35.315</f>
-        <v>0.59465128132521594</v>
+        <v>0.56633158714427301</v>
       </c>
       <c r="D4">
         <f>D3/35.315</f>
-        <v>0.59464881778281187</v>
+        <v>0.59464816650148666</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
@@ -3804,7 +4519,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
+      <c r="A6" s="27"/>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
@@ -3875,36 +4590,36 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>-4.1666679999999998E-2</v>
+        <v>4.1666269999999998E-2</v>
       </c>
       <c r="F13">
-        <v>-8.3331499999999992E-3</v>
+        <v>8.3331900000000007E-3</v>
       </c>
       <c r="G13">
         <f>E13/F13</f>
-        <v>5.0001116024552541</v>
+        <v>5.0000384006604905</v>
       </c>
       <c r="H13">
         <f>Constants!B6</f>
-        <v>1.8800000000000003E-8</v>
+        <v>0</v>
       </c>
       <c r="I13" s="5">
-        <v>500002.5</v>
+        <v>500007.5</v>
       </c>
       <c r="J13" s="5">
         <v>102.5</v>
       </c>
       <c r="K13" s="5">
-        <v>500000</v>
+        <v>500010</v>
       </c>
       <c r="L13" s="5">
         <v>102.5</v>
@@ -3919,9 +4634,6 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
-      <c r="P14" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="P15" t="s">
@@ -3967,25 +4679,25 @@
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>-4.1666679999999998E-2</v>
+        <v>4.1666269999999998E-2</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G19">
         <v>-1</v>
       </c>
       <c r="H19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P19" t="s">
         <v>59</v>
@@ -4024,8 +4736,8 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
       <c r="H36" s="6" t="s">
         <v>47</v>
       </c>
@@ -4041,17 +4753,17 @@
     <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B37" s="8">
         <f>D3/D5</f>
-        <v>7.0000076666666661E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="9">
         <f>C3/C5*C6</f>
-        <v>7.0000366666666665</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="F37" t="s">
         <v>44</v>
@@ -4061,551 +4773,17 @@
       </c>
       <c r="H37" s="6">
         <f>G13*H13/M13</f>
-        <v>3.7600839250463518E-8</v>
+        <v>0</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>45</v>
       </c>
       <c r="K37" s="6">
         <f>G13*H13/M13</f>
-        <v>3.7600839250463518E-8</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M37" t="s">
-        <v>45</v>
-      </c>
-      <c r="N37" s="7">
-        <f>E19*G19</f>
-        <v>4.1666679999999998E-2</v>
-      </c>
-      <c r="O37" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="P37" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-      <c r="E46">
-        <v>3</v>
-      </c>
-      <c r="F46">
-        <v>4</v>
-      </c>
-      <c r="G46">
-        <v>5</v>
-      </c>
-      <c r="H46">
-        <v>6</v>
-      </c>
-      <c r="I46">
-        <v>7</v>
-      </c>
-      <c r="M46" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8">
-        <f>B37</f>
-        <v>7.0000076666666661E-2</v>
-      </c>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7">
-        <f>N37</f>
-        <v>4.1666679999999998E-2</v>
-      </c>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>55</v>
-      </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>56</v>
-      </c>
-      <c r="B51">
-        <f>SUM(B47:B49)</f>
-        <v>0</v>
-      </c>
-      <c r="C51">
-        <f t="shared" ref="C51:I51" si="0">SUM(C47:C49)</f>
-        <v>0</v>
-      </c>
-      <c r="D51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F51">
-        <f t="shared" si="0"/>
-        <v>0.11166675666666666</v>
-      </c>
-      <c r="G51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M51" s="10">
-        <f>E37</f>
-        <v>7.0000366666666665</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>65</v>
-      </c>
-      <c r="B52">
-        <f>B47+B48</f>
-        <v>0</v>
-      </c>
-      <c r="C52">
-        <f t="shared" ref="C52:I52" si="1">C47+C48</f>
-        <v>0</v>
-      </c>
-      <c r="D52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F52">
-        <f t="shared" si="1"/>
-        <v>0.11166675666666666</v>
-      </c>
-      <c r="G52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I52">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M52">
-        <f>E37</f>
-        <v>7.0000366666666665</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="B36:C36"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F1D4CD-3FDB-4235-A1C3-31288C66CE2D}">
-  <dimension ref="A1:P52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.90625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
-      <c r="B3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3">
-        <v>21</v>
-      </c>
-      <c r="D3">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
-      <c r="B4" s="8"/>
-      <c r="C4">
-        <f>C3/35.315</f>
-        <v>0.59464816650148666</v>
-      </c>
-      <c r="D4">
-        <f>D3/35.315</f>
-        <v>0.59464816650148666</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
-      <c r="B5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>300</v>
-      </c>
-      <c r="D5">
-        <v>300</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
-      <c r="B6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" s="20" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="21"/>
-      <c r="E11" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B12" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="E13">
-        <v>4.1666269999999998E-2</v>
-      </c>
-      <c r="F13">
-        <v>8.3331900000000007E-3</v>
-      </c>
-      <c r="G13">
-        <f>E13/F13</f>
-        <v>5.0000384006604905</v>
-      </c>
-      <c r="H13">
-        <f>Constants!B6</f>
-        <v>1.8800000000000003E-8</v>
-      </c>
-      <c r="I13" s="5">
-        <v>500007.5</v>
-      </c>
-      <c r="J13" s="5">
-        <v>102.5</v>
-      </c>
-      <c r="K13" s="5">
-        <v>500010</v>
-      </c>
-      <c r="L13" s="5">
-        <v>102.5</v>
-      </c>
-      <c r="M13">
-        <f>SQRT((K13-I13)^2-(L13-J13)^2)</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="P15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="E17" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="P17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B18" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="F18" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="P18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>6</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-      <c r="E19">
-        <v>4.1666269999999998E-2</v>
-      </c>
-      <c r="F19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19">
-        <v>-1</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="P19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="P20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="P21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="H22" s="3"/>
-      <c r="P22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="25" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="27" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="29" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="30" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="2:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="H35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="H36" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="N36" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="O36" s="7"/>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B37" s="8">
-        <f>D3/D5</f>
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="9">
-        <f>C3/C5*C6</f>
-        <v>7.0000000000000009</v>
-      </c>
-      <c r="F37" t="s">
-        <v>44</v>
-      </c>
-      <c r="G37" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" s="6">
-        <f>G13*H13/M13</f>
-        <v>3.7600288772966896E-8</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K37" s="6">
-        <f>G13*H13/M13</f>
-        <v>3.7600288772966896E-8</v>
+        <v>0</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>7</v>
@@ -4698,12 +4876,18 @@
         <v>55</v>
       </c>
       <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
+      <c r="C49" s="6">
+        <f>-H37</f>
+        <v>0</v>
+      </c>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
+      <c r="H49" s="6">
+        <f>K37</f>
+        <v>0</v>
+      </c>
       <c r="I49" s="6"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
@@ -4744,7 +4928,7 @@
       </c>
       <c r="M51" s="10">
         <f>E37</f>
-        <v>7.0000000000000009</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
@@ -4785,7 +4969,7 @@
       </c>
       <c r="M52">
         <f>E37</f>
-        <v>7.0000000000000009</v>
+        <v>6.666666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -4800,29 +4984,35 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8666B46-C872-40BF-8072-9D3544872922}">
-  <dimension ref="B1:Z19"/>
+  <dimension ref="B1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5"/>
+    <sheetView topLeftCell="J7" zoomScale="95" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="6" max="10" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.36328125" customWidth="1"/>
+    <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.54296875" customWidth="1"/>
+    <col min="26" max="26" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+    <row r="1" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="1"/>
       <c r="K1" s="2"/>
       <c r="L1" s="1" t="s">
@@ -4835,7 +5025,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C2" s="3">
         <v>0</v>
       </c>
@@ -4867,7 +5057,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3">
         <v>0</v>
       </c>
@@ -4921,12 +5111,12 @@
         <f>N3-S3</f>
         <v>7.6933333333251142E-4</v>
       </c>
-      <c r="W3" s="29">
+      <c r="W3" s="26">
         <f>N3/S3 - 1</f>
         <v>9.2318308728467358E-5</v>
       </c>
     </row>
-    <row r="4" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3">
         <v>1</v>
       </c>
@@ -4979,12 +5169,12 @@
         <f t="shared" ref="V4:V10" si="0">N4-S4</f>
         <v>8.7599999999987688E-4</v>
       </c>
-      <c r="W4" s="29">
-        <f t="shared" ref="W4:W10" si="1">N4/S4 - 1</f>
+      <c r="W4" s="26">
+        <f t="shared" ref="W4:W9" si="1">N4/S4 - 1</f>
         <v>1.0511941974078454E-4</v>
       </c>
     </row>
-    <row r="5" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>2</v>
       </c>
@@ -5028,9 +5218,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W5" s="29"/>
-    </row>
-    <row r="6" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W5" s="26"/>
+    </row>
+    <row r="6" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -5074,9 +5264,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W6" s="29"/>
-    </row>
-    <row r="7" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W6" s="26"/>
+    </row>
+    <row r="7" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>4</v>
       </c>
@@ -5122,12 +5312,12 @@
         <f t="shared" si="0"/>
         <v>2.7666666666092965E-5</v>
       </c>
-      <c r="W7" s="29">
+      <c r="W7" s="26">
         <f t="shared" si="1"/>
         <v>2.477609943429826E-6</v>
       </c>
     </row>
-    <row r="8" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>5</v>
       </c>
@@ -5171,9 +5361,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W8" s="29"/>
-    </row>
-    <row r="9" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W8" s="26"/>
+    </row>
+    <row r="9" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>6</v>
       </c>
@@ -5196,7 +5386,7 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="25">
         <v>0.11166626440000001</v>
       </c>
       <c r="J9">
@@ -5205,9 +5395,9 @@
       <c r="L9" t="s">
         <v>7</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9">
         <f>'Cell 6'!M51</f>
-        <v>7.0000000000000009</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="R9">
         <v>100</v>
@@ -5217,17 +5407,17 @@
       </c>
       <c r="V9">
         <f t="shared" si="0"/>
-        <v>5.6000000103750835E-7</v>
-      </c>
-      <c r="W9" s="29">
+        <v>-0.33333277333333289</v>
+      </c>
+      <c r="W9" s="26">
         <f t="shared" si="1"/>
-        <v>8.000000661922968E-8</v>
-      </c>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-    </row>
-    <row r="10" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>-4.7618971428565304E-2</v>
+      </c>
+      <c r="X9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>7</v>
       </c>
@@ -5271,12 +5461,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W10" s="29"/>
-    </row>
-    <row r="11" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="V11" s="28"/>
-    </row>
-    <row r="12" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="W10" s="26"/>
+    </row>
+    <row r="12" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>2</v>
       </c>
@@ -5285,7 +5472,7 @@
         <v>100.00623717684918</v>
       </c>
     </row>
-    <row r="13" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>3</v>
       </c>
@@ -5300,15 +5487,18 @@
         <f>(12.5+21.00011)/300*100</f>
         <v>11.166703333333333</v>
       </c>
-    </row>
-    <row r="14" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>1</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
-      <c r="M14" s="27"/>
+      <c r="M14" s="25"/>
       <c r="N14" t="s">
         <v>74</v>
       </c>
@@ -5316,8 +5506,11 @@
         <f>12.49987932/300</f>
         <v>4.16662644E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -5325,7 +5518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:26" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>5</v>
       </c>
@@ -5346,7 +5539,7 @@
         <v>7</v>
       </c>
       <c r="E18">
-        <v>100.00339567856261</v>
+        <v>97.018310298261014</v>
       </c>
     </row>
     <row r="19" spans="4:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -5379,16 +5572,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="1"/>
       <c r="K1" s="2"/>
       <c r="L1" s="1" t="s">

</xml_diff>

<commit_message>
updates for sumwere creek
some testing code for sumwere creek
</commit_message>
<xml_diff>
--- a/examples/dev_sandbox/data/mini_grid/placing_matrix_all_components_redo.xlsx
+++ b/examples/dev_sandbox/data/mini_grid/placing_matrix_all_components_redo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjordan\Documents\GitHub\ClearWater-riverine\examples\dev_sandbox\data\mini_grid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B36BAC4-1BA2-4405-B519-8F2220A451A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA30BFA-DE21-4722-BC6D-CAE1C2B625A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14490" yWindow="-18120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{0D6685A3-9F3A-4630-99AF-4A1490A22806}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10360" activeTab="7" xr2:uid="{0D6685A3-9F3A-4630-99AF-4A1490A22806}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagram" sheetId="15" r:id="rId1"/>
@@ -20,14 +20,15 @@
     <sheet name="Cell 4" sheetId="16" r:id="rId5"/>
     <sheet name="Cell 6" sheetId="17" r:id="rId6"/>
     <sheet name="Matrix" sheetId="2" r:id="rId7"/>
-    <sheet name="Matrix-No-Diffusion" sheetId="13" r:id="rId8"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId9"/>
-    <sheet name="Delta T" sheetId="1" r:id="rId10"/>
-    <sheet name="Face Area" sheetId="4" r:id="rId11"/>
-    <sheet name="Distance Between Cells" sheetId="8" r:id="rId12"/>
-    <sheet name="Flow Across Face" sheetId="10" r:id="rId13"/>
-    <sheet name="Total-No-Diffusion" sheetId="7" r:id="rId14"/>
-    <sheet name="Total" sheetId="6" r:id="rId15"/>
+    <sheet name="Matrix-Real-Only" sheetId="19" r:id="rId8"/>
+    <sheet name="Matrix-No-Diffusion" sheetId="13" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId10"/>
+    <sheet name="Delta T" sheetId="1" r:id="rId11"/>
+    <sheet name="Face Area" sheetId="4" r:id="rId12"/>
+    <sheet name="Distance Between Cells" sheetId="8" r:id="rId13"/>
+    <sheet name="Flow Across Face" sheetId="10" r:id="rId14"/>
+    <sheet name="Total-No-Diffusion" sheetId="7" r:id="rId15"/>
+    <sheet name="Total" sheetId="6" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="94">
   <si>
     <t>n+1</t>
   </si>
@@ -601,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -643,14 +644,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,6 +1456,18 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094487B4-28D2-4B35-9AEF-1A41EBED104F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8500680-5B59-40AC-AB01-A466D4D431DD}">
   <dimension ref="B1:M9"/>
   <sheetViews>
@@ -1467,16 +1481,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -1623,7 +1637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0995DFA7-E61E-4ADC-BFF8-E39AADF9E9D6}">
   <dimension ref="B1:M9"/>
   <sheetViews>
@@ -1634,16 +1648,16 @@
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -1799,7 +1813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EEBBD86-2495-4984-B5F3-6D4DD628368B}">
   <dimension ref="B1:M9"/>
   <sheetViews>
@@ -1810,16 +1824,16 @@
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:13" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -1924,7 +1938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FED8B94-C086-4105-BBEE-59F985EE19AB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1936,7 +1950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCAC273-7DB2-44F4-A0A4-6FE5EDD8BB88}">
   <dimension ref="B1:W18"/>
   <sheetViews>
@@ -1947,16 +1961,16 @@
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:23" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -2348,7 +2362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38CA6E72-7372-4C3B-AD40-0CE7B3853F9B}">
   <dimension ref="B1:U18"/>
   <sheetViews>
@@ -2359,16 +2373,16 @@
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="2:21" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1" t="s">
         <v>9</v>
@@ -2803,8 +2817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5779220-0CA2-48BC-B882-E6E428182D5B}">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2862,15 +2876,15 @@
       <c r="B4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="32">
+      <c r="C4" s="30">
         <f>C3/35.315</f>
         <v>0.70799280758884331</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="30">
         <f>D3/35.315</f>
         <v>0.70793008636556709</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="30" t="s">
         <v>17</v>
       </c>
       <c r="J4" t="s">
@@ -2937,7 +2951,7 @@
         <f>K6-K7</f>
         <v>2.3079999999993106E-3</v>
       </c>
-      <c r="N8" s="31">
+      <c r="N8" s="29">
         <f>K8/300 *100</f>
         <v>7.6933333333310361E-4</v>
       </c>
@@ -3215,8 +3229,8 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
       <c r="H36" s="6" t="s">
         <v>47</v>
       </c>
@@ -3538,7 +3552,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="29"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
@@ -3563,17 +3577,17 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="29"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="32">
+      <c r="C4" s="30">
         <f>C3/35.315</f>
         <v>0.70799280758884331</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="30">
         <f>D3/35.315</f>
         <v>0.70791924111567328</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="30"/>
       <c r="J4" t="s">
         <v>75</v>
       </c>
@@ -3583,7 +3597,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
@@ -3605,7 +3619,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="29"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
@@ -3640,7 +3654,7 @@
         <f>K6-K7</f>
         <v>2.6280000000049597E-3</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="29">
         <f>K8/300*100</f>
         <v>8.7600000000165313E-4</v>
       </c>
@@ -3907,8 +3921,8 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
       <c r="H36" s="6" t="s">
         <v>47</v>
       </c>
@@ -4227,7 +4241,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A3" s="29"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
@@ -4257,17 +4271,17 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A4" s="29"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="32">
+      <c r="C4" s="30">
         <f>C3/35.315</f>
         <v>0.59465128132521594</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="30">
         <f>D3/35.315</f>
         <v>0.59464881778281187</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="30" t="s">
         <v>17</v>
       </c>
       <c r="L4" t="s">
@@ -4279,7 +4293,7 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
@@ -4307,7 +4321,7 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="29"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
@@ -4534,8 +4548,8 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
       <c r="H36" s="6" t="s">
         <v>47</v>
       </c>
@@ -4809,7 +4823,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="29"/>
+      <c r="A3" s="31"/>
       <c r="B3" s="8" t="s">
         <v>13</v>
       </c>
@@ -4837,17 +4851,17 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="29"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="32">
+      <c r="C4" s="30">
         <f>C3/35.315</f>
         <v>0.56633158714427301</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="30">
         <f>D3/35.315</f>
         <v>0.59464816650148666</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="30" t="s">
         <v>17</v>
       </c>
       <c r="L4" t="s">
@@ -4859,7 +4873,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="29"/>
+      <c r="A5" s="31"/>
       <c r="B5" s="8" t="s">
         <v>16</v>
       </c>
@@ -4881,7 +4895,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="29"/>
+      <c r="A6" s="31"/>
       <c r="B6" s="8" t="s">
         <v>20</v>
       </c>
@@ -5105,8 +5119,8 @@
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
       <c r="H36" s="6" t="s">
         <v>47</v>
       </c>
@@ -5355,8 +5369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8666B46-C872-40BF-8072-9D3544872922}">
   <dimension ref="B1:X19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView zoomScale="39" zoomScaleNormal="39" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5373,16 +5387,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="1"/>
       <c r="K1" s="2"/>
       <c r="L1" s="1" t="s">
@@ -5480,7 +5494,7 @@
         <f t="array" ref="S3:S10">MMULT(C3:J10, R3:R10)</f>
         <v>8.3334860000000006</v>
       </c>
-      <c r="V3" s="31">
+      <c r="V3" s="29">
         <f>N3-S3</f>
         <v>7.6933333333251142E-4</v>
       </c>
@@ -5541,7 +5555,7 @@
       <c r="S4">
         <v>8.3333793333333332</v>
       </c>
-      <c r="V4" s="31">
+      <c r="V4" s="29">
         <f t="shared" ref="V4:V10" si="0">N4-S4</f>
         <v>8.7599999999987688E-4</v>
       </c>
@@ -5935,6 +5949,571 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77DA86AA-3E67-4B13-ADA5-54D629D990C3}">
+  <dimension ref="B1:X19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.26953125" defaultRowHeight="45.5" customHeight="1" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="6" max="10" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="17" max="17" width="8.26953125" customWidth="1"/>
+    <col min="18" max="18" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.81640625" customWidth="1"/>
+    <col min="22" max="22" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.54296875" customWidth="1"/>
+    <col min="26" max="26" width="11.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1">
+        <v>12.499917</v>
+      </c>
+    </row>
+    <row r="2" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>3</v>
+      </c>
+      <c r="G2" s="3">
+        <v>4</v>
+      </c>
+      <c r="H2" s="3">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3">
+        <v>6</v>
+      </c>
+      <c r="J2" s="3">
+        <v>7</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>'Cell 0'!B51</f>
+        <v>0.12800160672162686</v>
+      </c>
+      <c r="D3">
+        <f>'Cell 0'!C51</f>
+        <v>-1.0000220806447549E-3</v>
+      </c>
+      <c r="E3" s="30">
+        <f>'Cell 0'!D51</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="30">
+        <f>'Cell 0'!E51</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="30">
+        <f>'Cell 0'!F51</f>
+        <v>-4.3666724640982098E-2</v>
+      </c>
+      <c r="H3" s="30">
+        <f>'Cell 0'!G51</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="30">
+        <f>'Cell 0'!H51</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="30">
+        <f>'Cell 0'!I51</f>
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <f>'Cell 0'!M51+(G3*-1*100)</f>
+        <v>12.700927797431543</v>
+      </c>
+      <c r="R3">
+        <v>100</v>
+      </c>
+      <c r="S3" cm="1">
+        <f t="array" ref="S3:S4">MMULT(C3:D4, R3:R4)</f>
+        <v>12.700158464098211</v>
+      </c>
+      <c r="V3" s="29">
+        <f>N3-S3</f>
+        <v>7.6933333333251142E-4</v>
+      </c>
+      <c r="W3" s="26">
+        <f>N3/S3 - 1</f>
+        <v>6.05766719767864E-5</v>
+      </c>
+      <c r="X3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <f>'Cell 1'!B51</f>
+        <v>-4.2666392080644759E-2</v>
+      </c>
+      <c r="D4">
+        <f>'Cell 1'!C51</f>
+        <v>0.12800020077424229</v>
+      </c>
+      <c r="E4" s="30">
+        <f>'Cell 1'!D51</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="30">
+        <f>'Cell 1'!E51</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="30">
+        <f>'Cell 1'!F51</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="30">
+        <f>'Cell 1'!G51</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="30">
+        <f>'Cell 1'!H51</f>
+        <v>-2.0000153602641965E-3</v>
+      </c>
+      <c r="J4" s="30">
+        <f>'Cell 1'!I51</f>
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <f>'Cell 1'!M51+(I4*-1*100)</f>
+        <v>8.5342568693597531</v>
+      </c>
+      <c r="R4">
+        <v>100</v>
+      </c>
+      <c r="S4">
+        <v>8.5333808693597533</v>
+      </c>
+      <c r="V4" s="29">
+        <f t="shared" ref="V4:V10" si="0">N4-S4</f>
+        <v>8.7599999999987688E-4</v>
+      </c>
+      <c r="W4" s="26">
+        <f t="shared" ref="W4:W9" si="1">N4/S4 - 1</f>
+        <v>1.0265567814338183E-4</v>
+      </c>
+      <c r="X4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="30">
+        <v>0</v>
+      </c>
+      <c r="D5" s="30">
+        <v>0</v>
+      </c>
+      <c r="E5" s="30">
+        <v>1</v>
+      </c>
+      <c r="F5" s="30">
+        <v>0</v>
+      </c>
+      <c r="G5" s="30">
+        <v>0</v>
+      </c>
+      <c r="H5" s="30">
+        <v>0</v>
+      </c>
+      <c r="I5" s="30">
+        <v>0</v>
+      </c>
+      <c r="J5" s="30">
+        <v>0</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30">
+        <v>0</v>
+      </c>
+      <c r="R5" s="30">
+        <v>0</v>
+      </c>
+      <c r="S5" s="30"/>
+      <c r="V5" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="33"/>
+    </row>
+    <row r="6" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="3">
+        <v>3</v>
+      </c>
+      <c r="C6" s="30">
+        <v>0</v>
+      </c>
+      <c r="D6" s="30">
+        <v>0</v>
+      </c>
+      <c r="E6" s="30">
+        <v>0</v>
+      </c>
+      <c r="F6" s="30">
+        <v>1</v>
+      </c>
+      <c r="G6" s="30">
+        <v>0</v>
+      </c>
+      <c r="H6" s="30">
+        <v>0</v>
+      </c>
+      <c r="I6" s="30">
+        <v>0</v>
+      </c>
+      <c r="J6" s="30">
+        <v>0</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30">
+        <v>0</v>
+      </c>
+      <c r="R6" s="30">
+        <v>0</v>
+      </c>
+      <c r="S6" s="30"/>
+      <c r="V6" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W6" s="33"/>
+    </row>
+    <row r="7" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="3">
+        <v>4</v>
+      </c>
+      <c r="C7" s="30" cm="1">
+        <f t="array" ref="C7:J7">'Cell 4'!B51:I51</f>
+        <v>-2.0000446409821015E-3</v>
+      </c>
+      <c r="D7" s="30">
+        <v>0</v>
+      </c>
+      <c r="E7" s="30">
+        <v>0</v>
+      </c>
+      <c r="F7" s="30">
+        <v>0</v>
+      </c>
+      <c r="G7" s="30">
+        <v>0.11366680130764877</v>
+      </c>
+      <c r="H7" s="30">
+        <v>0</v>
+      </c>
+      <c r="I7" s="30">
+        <v>0</v>
+      </c>
+      <c r="J7" s="30">
+        <v>0</v>
+      </c>
+      <c r="L7" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30">
+        <f>(12.499917+21.00011)/300*100</f>
+        <v>11.166675666666666</v>
+      </c>
+      <c r="R7" s="30">
+        <v>100</v>
+      </c>
+      <c r="S7" s="30"/>
+      <c r="V7" s="30">
+        <f t="shared" si="0"/>
+        <v>11.166675666666666</v>
+      </c>
+      <c r="W7" s="33" t="e">
+        <f t="shared" ref="W7:W12" si="2">N7/S7 - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="3">
+        <v>5</v>
+      </c>
+      <c r="C8" s="30">
+        <v>0</v>
+      </c>
+      <c r="D8" s="30">
+        <v>0</v>
+      </c>
+      <c r="E8" s="30">
+        <v>0</v>
+      </c>
+      <c r="F8" s="30">
+        <v>0</v>
+      </c>
+      <c r="G8" s="30">
+        <v>0</v>
+      </c>
+      <c r="H8" s="30">
+        <v>1</v>
+      </c>
+      <c r="I8" s="30">
+        <v>0</v>
+      </c>
+      <c r="J8" s="30">
+        <v>0</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30">
+        <v>0</v>
+      </c>
+      <c r="R8" s="30">
+        <v>0</v>
+      </c>
+      <c r="S8" s="30"/>
+      <c r="V8" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="33"/>
+    </row>
+    <row r="9" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="3">
+        <v>6</v>
+      </c>
+      <c r="C9" s="30" cm="1">
+        <f t="array" ref="C9:J9">'Cell 6'!B51:I51</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="30">
+        <v>-4.3666285360264193E-2</v>
+      </c>
+      <c r="E9" s="30">
+        <v>0</v>
+      </c>
+      <c r="F9" s="30">
+        <v>0</v>
+      </c>
+      <c r="G9" s="30">
+        <v>0</v>
+      </c>
+      <c r="H9" s="30">
+        <v>0</v>
+      </c>
+      <c r="I9" s="30">
+        <v>0.11033295202693087</v>
+      </c>
+      <c r="J9" s="30">
+        <v>0</v>
+      </c>
+      <c r="L9" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30">
+        <f>'Cell 6'!M51</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="R9" s="30">
+        <v>100</v>
+      </c>
+      <c r="S9" s="30"/>
+      <c r="V9" s="30">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="W9" s="33" t="e">
+        <f t="shared" ref="W9:W14" si="3">N9/S9 - 1</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="3">
+        <v>7</v>
+      </c>
+      <c r="C10" s="30">
+        <v>0</v>
+      </c>
+      <c r="D10" s="30">
+        <v>0</v>
+      </c>
+      <c r="E10" s="30">
+        <v>0</v>
+      </c>
+      <c r="F10" s="30">
+        <v>0</v>
+      </c>
+      <c r="G10" s="30">
+        <v>0</v>
+      </c>
+      <c r="H10" s="30">
+        <v>0</v>
+      </c>
+      <c r="I10" s="30">
+        <v>0</v>
+      </c>
+      <c r="J10" s="30">
+        <v>1</v>
+      </c>
+      <c r="L10" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30">
+        <v>0</v>
+      </c>
+      <c r="R10" s="30">
+        <v>0</v>
+      </c>
+      <c r="S10" s="30"/>
+      <c r="V10" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W10" s="33"/>
+    </row>
+    <row r="12" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" cm="1">
+        <f t="array" ref="E12:E13">MMULT(MINVERSE(C3:D4), N3:N4)</f>
+        <v>100.00607964086643</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>100.00887026999997</v>
+      </c>
+      <c r="M13" s="4"/>
+      <c r="N13" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q13">
+        <f>N7</f>
+        <v>11.166675666666666</v>
+      </c>
+      <c r="R13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="M14" s="25"/>
+      <c r="N14" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q14">
+        <f>'Cell 6'!M6</f>
+        <v>3.8332936666666664E-2</v>
+      </c>
+      <c r="R14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="30"/>
+    </row>
+    <row r="16" spans="2:24" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="30"/>
+    </row>
+    <row r="17" spans="4:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="30"/>
+    </row>
+    <row r="18" spans="4:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="30"/>
+    </row>
+    <row r="19" spans="4:5" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B87C51-26FD-476D-A4AB-4D8217DA3413}">
   <dimension ref="B1:N18"/>
   <sheetViews>
@@ -5948,16 +6527,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="45.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
       <c r="J1" s="1"/>
       <c r="K1" s="2"/>
       <c r="L1" s="1" t="s">
@@ -6144,16 +6723,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{094487B4-28D2-4B35-9AEF-1A41EBED104F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>